<commit_message>
F03 Froze Encoder 1
</commit_message>
<xml_diff>
--- a/Epoch Accuracy.xlsx
+++ b/Epoch Accuracy.xlsx
@@ -424,7 +424,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:B114"/>
+  <dimension ref="A2:B118"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:B114"/>
@@ -437,7 +437,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>0.984375</v>
+        <v>0.96875</v>
       </c>
     </row>
     <row r="3">
@@ -445,7 +445,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>0.984375</v>
+        <v>0.953125</v>
       </c>
     </row>
     <row r="4">
@@ -453,7 +453,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>0.96875</v>
+        <v>0.984375</v>
       </c>
     </row>
     <row r="5">
@@ -461,7 +461,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>0.984375</v>
+        <v>0.9375</v>
       </c>
     </row>
     <row r="6">
@@ -469,7 +469,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>0.953125</v>
+        <v>0.921875</v>
       </c>
     </row>
     <row r="7">
@@ -477,7 +477,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>0.9375</v>
+        <v>0.859375</v>
       </c>
     </row>
     <row r="8">
@@ -485,7 +485,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>0.9375</v>
+        <v>0.859375</v>
       </c>
     </row>
     <row r="9">
@@ -493,7 +493,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>0.953125</v>
+        <v>0.8125</v>
       </c>
     </row>
     <row r="10">
@@ -501,7 +501,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>0.96875</v>
+        <v>0.859375</v>
       </c>
     </row>
     <row r="11">
@@ -509,7 +509,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>0.96875</v>
+        <v>0.875</v>
       </c>
     </row>
     <row r="12">
@@ -517,7 +517,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>0.953125</v>
+        <v>0.859375</v>
       </c>
     </row>
     <row r="13">
@@ -525,7 +525,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>0.953125</v>
+        <v>0.859375</v>
       </c>
     </row>
     <row r="14">
@@ -533,7 +533,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>0.9375</v>
+        <v>0.84375</v>
       </c>
     </row>
     <row r="15">
@@ -541,7 +541,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>0.953125</v>
+        <v>0.828125</v>
       </c>
     </row>
     <row r="16">
@@ -549,7 +549,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>0.90625</v>
+        <v>0.796875</v>
       </c>
     </row>
     <row r="17">
@@ -557,7 +557,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>0.90625</v>
+        <v>0.796875</v>
       </c>
     </row>
     <row r="18">
@@ -565,7 +565,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>0.9375</v>
+        <v>0.8125</v>
       </c>
     </row>
     <row r="19">
@@ -573,7 +573,7 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>0.96875</v>
+        <v>0.796875</v>
       </c>
     </row>
     <row r="20">
@@ -581,7 +581,7 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>0.9375</v>
+        <v>0.78125</v>
       </c>
     </row>
     <row r="21">
@@ -589,7 +589,7 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>0.921875</v>
+        <v>0.78125</v>
       </c>
     </row>
     <row r="22">
@@ -597,7 +597,7 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>0.921875</v>
+        <v>0.78125</v>
       </c>
     </row>
     <row r="23">
@@ -605,7 +605,7 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>0.921875</v>
+        <v>0.765625</v>
       </c>
     </row>
     <row r="24">
@@ -613,7 +613,7 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>0.890625</v>
+        <v>0.765625</v>
       </c>
     </row>
     <row r="25">
@@ -621,7 +621,7 @@
         <v>23</v>
       </c>
       <c r="B25" t="n">
-        <v>0.90625</v>
+        <v>0.78125</v>
       </c>
     </row>
     <row r="26">
@@ -629,7 +629,7 @@
         <v>24</v>
       </c>
       <c r="B26" t="n">
-        <v>0.875</v>
+        <v>0.78125</v>
       </c>
     </row>
     <row r="27">
@@ -637,7 +637,7 @@
         <v>25</v>
       </c>
       <c r="B27" t="n">
-        <v>0.859375</v>
+        <v>0.78125</v>
       </c>
     </row>
     <row r="28">
@@ -645,7 +645,7 @@
         <v>26</v>
       </c>
       <c r="B28" t="n">
-        <v>0.875</v>
+        <v>0.78125</v>
       </c>
     </row>
     <row r="29">
@@ -653,7 +653,7 @@
         <v>27</v>
       </c>
       <c r="B29" t="n">
-        <v>0.875</v>
+        <v>0.78125</v>
       </c>
     </row>
     <row r="30">
@@ -661,7 +661,7 @@
         <v>28</v>
       </c>
       <c r="B30" t="n">
-        <v>0.875</v>
+        <v>0.78125</v>
       </c>
     </row>
     <row r="31">
@@ -669,7 +669,7 @@
         <v>29</v>
       </c>
       <c r="B31" t="n">
-        <v>0.875</v>
+        <v>0.796875</v>
       </c>
     </row>
     <row r="32">
@@ -677,7 +677,7 @@
         <v>30</v>
       </c>
       <c r="B32" t="n">
-        <v>0.875</v>
+        <v>0.796875</v>
       </c>
     </row>
     <row r="33">
@@ -685,7 +685,7 @@
         <v>31</v>
       </c>
       <c r="B33" t="n">
-        <v>0.875</v>
+        <v>0.796875</v>
       </c>
     </row>
     <row r="34">
@@ -693,7 +693,7 @@
         <v>32</v>
       </c>
       <c r="B34" t="n">
-        <v>0.875</v>
+        <v>0.796875</v>
       </c>
     </row>
     <row r="35">
@@ -701,7 +701,7 @@
         <v>33</v>
       </c>
       <c r="B35" t="n">
-        <v>0.875</v>
+        <v>0.796875</v>
       </c>
     </row>
     <row r="36">
@@ -709,7 +709,7 @@
         <v>34</v>
       </c>
       <c r="B36" t="n">
-        <v>0.859375</v>
+        <v>0.796875</v>
       </c>
     </row>
     <row r="37">
@@ -717,7 +717,7 @@
         <v>35</v>
       </c>
       <c r="B37" t="n">
-        <v>0.859375</v>
+        <v>0.796875</v>
       </c>
     </row>
     <row r="38">
@@ -725,7 +725,7 @@
         <v>36</v>
       </c>
       <c r="B38" t="n">
-        <v>0.859375</v>
+        <v>0.796875</v>
       </c>
     </row>
     <row r="39">
@@ -733,7 +733,7 @@
         <v>37</v>
       </c>
       <c r="B39" t="n">
-        <v>0.875</v>
+        <v>0.796875</v>
       </c>
     </row>
     <row r="40">
@@ -741,7 +741,7 @@
         <v>38</v>
       </c>
       <c r="B40" t="n">
-        <v>0.875</v>
+        <v>0.796875</v>
       </c>
     </row>
     <row r="41">
@@ -749,7 +749,7 @@
         <v>39</v>
       </c>
       <c r="B41" t="n">
-        <v>0.875</v>
+        <v>0.796875</v>
       </c>
     </row>
     <row r="42">
@@ -757,7 +757,7 @@
         <v>40</v>
       </c>
       <c r="B42" t="n">
-        <v>0.875</v>
+        <v>0.796875</v>
       </c>
     </row>
     <row r="43">
@@ -765,7 +765,7 @@
         <v>41</v>
       </c>
       <c r="B43" t="n">
-        <v>0.890625</v>
+        <v>0.796875</v>
       </c>
     </row>
     <row r="44">
@@ -773,7 +773,7 @@
         <v>42</v>
       </c>
       <c r="B44" t="n">
-        <v>0.890625</v>
+        <v>0.796875</v>
       </c>
     </row>
     <row r="45">
@@ -781,7 +781,7 @@
         <v>43</v>
       </c>
       <c r="B45" t="n">
-        <v>0.890625</v>
+        <v>0.796875</v>
       </c>
     </row>
     <row r="46">
@@ -789,7 +789,7 @@
         <v>44</v>
       </c>
       <c r="B46" t="n">
-        <v>0.890625</v>
+        <v>0.8125</v>
       </c>
     </row>
     <row r="47">
@@ -797,7 +797,7 @@
         <v>45</v>
       </c>
       <c r="B47" t="n">
-        <v>0.890625</v>
+        <v>0.8125</v>
       </c>
     </row>
     <row r="48">
@@ -805,7 +805,7 @@
         <v>46</v>
       </c>
       <c r="B48" t="n">
-        <v>0.890625</v>
+        <v>0.796875</v>
       </c>
     </row>
     <row r="49">
@@ -813,7 +813,7 @@
         <v>47</v>
       </c>
       <c r="B49" t="n">
-        <v>0.890625</v>
+        <v>0.796875</v>
       </c>
     </row>
     <row r="50">
@@ -821,7 +821,7 @@
         <v>48</v>
       </c>
       <c r="B50" t="n">
-        <v>0.890625</v>
+        <v>0.796875</v>
       </c>
     </row>
     <row r="51">
@@ -829,7 +829,7 @@
         <v>49</v>
       </c>
       <c r="B51" t="n">
-        <v>0.890625</v>
+        <v>0.796875</v>
       </c>
     </row>
     <row r="52">
@@ -837,7 +837,7 @@
         <v>50</v>
       </c>
       <c r="B52" t="n">
-        <v>0.890625</v>
+        <v>0.796875</v>
       </c>
     </row>
     <row r="53">
@@ -845,7 +845,7 @@
         <v>51</v>
       </c>
       <c r="B53" t="n">
-        <v>0.890625</v>
+        <v>0.796875</v>
       </c>
     </row>
     <row r="54">
@@ -853,7 +853,7 @@
         <v>52</v>
       </c>
       <c r="B54" t="n">
-        <v>0.890625</v>
+        <v>0.796875</v>
       </c>
     </row>
     <row r="55">
@@ -861,7 +861,7 @@
         <v>53</v>
       </c>
       <c r="B55" t="n">
-        <v>0.90625</v>
+        <v>0.796875</v>
       </c>
     </row>
     <row r="56">
@@ -869,7 +869,7 @@
         <v>54</v>
       </c>
       <c r="B56" t="n">
-        <v>0.90625</v>
+        <v>0.796875</v>
       </c>
     </row>
     <row r="57">
@@ -877,7 +877,7 @@
         <v>55</v>
       </c>
       <c r="B57" t="n">
-        <v>0.90625</v>
+        <v>0.796875</v>
       </c>
     </row>
     <row r="58">
@@ -885,7 +885,7 @@
         <v>56</v>
       </c>
       <c r="B58" t="n">
-        <v>0.90625</v>
+        <v>0.796875</v>
       </c>
     </row>
     <row r="59">
@@ -893,7 +893,7 @@
         <v>57</v>
       </c>
       <c r="B59" t="n">
-        <v>0.90625</v>
+        <v>0.796875</v>
       </c>
     </row>
     <row r="60">
@@ -901,7 +901,7 @@
         <v>58</v>
       </c>
       <c r="B60" t="n">
-        <v>0.90625</v>
+        <v>0.796875</v>
       </c>
     </row>
     <row r="61">
@@ -909,7 +909,7 @@
         <v>59</v>
       </c>
       <c r="B61" t="n">
-        <v>0.921875</v>
+        <v>0.796875</v>
       </c>
     </row>
     <row r="62">
@@ -917,7 +917,7 @@
         <v>60</v>
       </c>
       <c r="B62" t="n">
-        <v>0.90625</v>
+        <v>0.796875</v>
       </c>
     </row>
     <row r="63">
@@ -925,7 +925,7 @@
         <v>61</v>
       </c>
       <c r="B63" t="n">
-        <v>0.90625</v>
+        <v>0.796875</v>
       </c>
     </row>
     <row r="64">
@@ -933,7 +933,7 @@
         <v>62</v>
       </c>
       <c r="B64" t="n">
-        <v>0.90625</v>
+        <v>0.796875</v>
       </c>
     </row>
     <row r="65">
@@ -941,7 +941,7 @@
         <v>63</v>
       </c>
       <c r="B65" t="n">
-        <v>0.921875</v>
+        <v>0.796875</v>
       </c>
     </row>
     <row r="66">
@@ -949,7 +949,7 @@
         <v>64</v>
       </c>
       <c r="B66" t="n">
-        <v>0.921875</v>
+        <v>0.796875</v>
       </c>
     </row>
     <row r="67">
@@ -957,7 +957,7 @@
         <v>65</v>
       </c>
       <c r="B67" t="n">
-        <v>0.921875</v>
+        <v>0.796875</v>
       </c>
     </row>
     <row r="68">
@@ -965,7 +965,7 @@
         <v>66</v>
       </c>
       <c r="B68" t="n">
-        <v>0.921875</v>
+        <v>0.8125</v>
       </c>
     </row>
     <row r="69">
@@ -973,7 +973,7 @@
         <v>67</v>
       </c>
       <c r="B69" t="n">
-        <v>0.921875</v>
+        <v>0.8125</v>
       </c>
     </row>
     <row r="70">
@@ -981,7 +981,7 @@
         <v>68</v>
       </c>
       <c r="B70" t="n">
-        <v>0.921875</v>
+        <v>0.8125</v>
       </c>
     </row>
     <row r="71">
@@ -989,7 +989,7 @@
         <v>69</v>
       </c>
       <c r="B71" t="n">
-        <v>0.9375</v>
+        <v>0.8125</v>
       </c>
     </row>
     <row r="72">
@@ -997,7 +997,7 @@
         <v>70</v>
       </c>
       <c r="B72" t="n">
-        <v>0.9375</v>
+        <v>0.8125</v>
       </c>
     </row>
     <row r="73">
@@ -1005,7 +1005,7 @@
         <v>71</v>
       </c>
       <c r="B73" t="n">
-        <v>0.9375</v>
+        <v>0.8125</v>
       </c>
     </row>
     <row r="74">
@@ -1013,7 +1013,7 @@
         <v>72</v>
       </c>
       <c r="B74" t="n">
-        <v>0.9375</v>
+        <v>0.796875</v>
       </c>
     </row>
     <row r="75">
@@ -1021,7 +1021,7 @@
         <v>73</v>
       </c>
       <c r="B75" t="n">
-        <v>0.9375</v>
+        <v>0.796875</v>
       </c>
     </row>
     <row r="76">
@@ -1029,7 +1029,7 @@
         <v>74</v>
       </c>
       <c r="B76" t="n">
-        <v>0.9375</v>
+        <v>0.796875</v>
       </c>
     </row>
     <row r="77">
@@ -1037,7 +1037,7 @@
         <v>75</v>
       </c>
       <c r="B77" t="n">
-        <v>0.9375</v>
+        <v>0.796875</v>
       </c>
     </row>
     <row r="78">
@@ -1045,7 +1045,7 @@
         <v>76</v>
       </c>
       <c r="B78" t="n">
-        <v>0.9375</v>
+        <v>0.796875</v>
       </c>
     </row>
     <row r="79">
@@ -1053,7 +1053,7 @@
         <v>77</v>
       </c>
       <c r="B79" t="n">
-        <v>0.9375</v>
+        <v>0.796875</v>
       </c>
     </row>
     <row r="80">
@@ -1061,7 +1061,7 @@
         <v>78</v>
       </c>
       <c r="B80" t="n">
-        <v>0.9375</v>
+        <v>0.796875</v>
       </c>
     </row>
     <row r="81">
@@ -1069,7 +1069,7 @@
         <v>79</v>
       </c>
       <c r="B81" t="n">
-        <v>0.9375</v>
+        <v>0.796875</v>
       </c>
     </row>
     <row r="82">
@@ -1077,7 +1077,7 @@
         <v>80</v>
       </c>
       <c r="B82" t="n">
-        <v>0.9375</v>
+        <v>0.796875</v>
       </c>
     </row>
     <row r="83">
@@ -1085,7 +1085,7 @@
         <v>81</v>
       </c>
       <c r="B83" t="n">
-        <v>0.9375</v>
+        <v>0.796875</v>
       </c>
     </row>
     <row r="84">
@@ -1093,7 +1093,7 @@
         <v>82</v>
       </c>
       <c r="B84" t="n">
-        <v>0.9375</v>
+        <v>0.796875</v>
       </c>
     </row>
     <row r="85">
@@ -1101,7 +1101,7 @@
         <v>83</v>
       </c>
       <c r="B85" t="n">
-        <v>0.9375</v>
+        <v>0.796875</v>
       </c>
     </row>
     <row r="86">
@@ -1109,7 +1109,7 @@
         <v>84</v>
       </c>
       <c r="B86" t="n">
-        <v>0.9375</v>
+        <v>0.796875</v>
       </c>
     </row>
     <row r="87">
@@ -1117,7 +1117,7 @@
         <v>85</v>
       </c>
       <c r="B87" t="n">
-        <v>0.9375</v>
+        <v>0.796875</v>
       </c>
     </row>
     <row r="88">
@@ -1125,7 +1125,7 @@
         <v>86</v>
       </c>
       <c r="B88" t="n">
-        <v>0.9375</v>
+        <v>0.796875</v>
       </c>
     </row>
     <row r="89">
@@ -1133,7 +1133,7 @@
         <v>87</v>
       </c>
       <c r="B89" t="n">
-        <v>0.9375</v>
+        <v>0.796875</v>
       </c>
     </row>
     <row r="90">
@@ -1141,7 +1141,7 @@
         <v>88</v>
       </c>
       <c r="B90" t="n">
-        <v>0.9375</v>
+        <v>0.796875</v>
       </c>
     </row>
     <row r="91">
@@ -1149,7 +1149,7 @@
         <v>89</v>
       </c>
       <c r="B91" t="n">
-        <v>0.9375</v>
+        <v>0.796875</v>
       </c>
     </row>
     <row r="92">
@@ -1157,7 +1157,7 @@
         <v>90</v>
       </c>
       <c r="B92" t="n">
-        <v>0.9375</v>
+        <v>0.796875</v>
       </c>
     </row>
     <row r="93">
@@ -1165,7 +1165,7 @@
         <v>91</v>
       </c>
       <c r="B93" t="n">
-        <v>0.9375</v>
+        <v>0.796875</v>
       </c>
     </row>
     <row r="94">
@@ -1173,7 +1173,7 @@
         <v>92</v>
       </c>
       <c r="B94" t="n">
-        <v>0.9375</v>
+        <v>0.796875</v>
       </c>
     </row>
     <row r="95">
@@ -1181,7 +1181,7 @@
         <v>93</v>
       </c>
       <c r="B95" t="n">
-        <v>0.9375</v>
+        <v>0.796875</v>
       </c>
     </row>
     <row r="96">
@@ -1189,7 +1189,7 @@
         <v>94</v>
       </c>
       <c r="B96" t="n">
-        <v>0.9375</v>
+        <v>0.796875</v>
       </c>
     </row>
     <row r="97">
@@ -1197,7 +1197,7 @@
         <v>95</v>
       </c>
       <c r="B97" t="n">
-        <v>0.9375</v>
+        <v>0.8125</v>
       </c>
     </row>
     <row r="98">
@@ -1205,7 +1205,7 @@
         <v>96</v>
       </c>
       <c r="B98" t="n">
-        <v>0.9375</v>
+        <v>0.8125</v>
       </c>
     </row>
     <row r="99">
@@ -1213,7 +1213,7 @@
         <v>97</v>
       </c>
       <c r="B99" t="n">
-        <v>0.9375</v>
+        <v>0.8125</v>
       </c>
     </row>
     <row r="100">
@@ -1221,7 +1221,7 @@
         <v>98</v>
       </c>
       <c r="B100" t="n">
-        <v>0.9375</v>
+        <v>0.8125</v>
       </c>
     </row>
     <row r="101">
@@ -1229,137 +1229,177 @@
         <v>99</v>
       </c>
       <c r="B101" t="n">
-        <v>0.9375</v>
+        <v>0.8125</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>&lt;__main__.DisplayOutputs object at 0x7f38b41323d0&gt;</t>
+          <t>&lt;__main__.DisplayOutputs object at 0x7fcda8314e50&gt;</t>
         </is>
       </c>
       <c r="B102" t="n">
-        <v>0.9375</v>
+        <v>0.8125</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>&lt;__main__.DisplayOutputs object at 0x7f38b41323d0&gt;</t>
+          <t>&lt;__main__.DisplayOutputs object at 0x7fcda8314e50&gt;</t>
         </is>
       </c>
       <c r="B103" t="n">
-        <v>0.953125</v>
+        <v>0.8125</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>&lt;__main__.DisplayOutputs object at 0x7f38b41323d0&gt;</t>
+          <t>&lt;__main__.DisplayOutputs object at 0x7fcda8314e50&gt;</t>
         </is>
       </c>
       <c r="B104" t="n">
-        <v>0.9375</v>
+        <v>0.734375</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>&lt;__main__.DisplayOutputs object at 0x7f38b41323d0&gt;</t>
+          <t>&lt;__main__.DisplayOutputs object at 0x7fcda8314e50&gt;</t>
         </is>
       </c>
       <c r="B105" t="n">
-        <v>0.90625</v>
+        <v>0.78125</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>&lt;__main__.DisplayOutputs object at 0x7f38b41323d0&gt;</t>
+          <t>&lt;__main__.DisplayOutputs object at 0x7fcda8314e50&gt;</t>
         </is>
       </c>
       <c r="B106" t="n">
-        <v>0.96875</v>
+        <v>0.84375</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>&lt;__main__.DisplayOutputs object at 0x7f38b41323d0&gt;</t>
+          <t>&lt;__main__.DisplayOutputs object at 0x7fcda8314e50&gt;</t>
         </is>
       </c>
       <c r="B107" t="n">
-        <v>0.96875</v>
+        <v>0.734375</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>&lt;__main__.DisplayOutputs object at 0x7f38b41323d0&gt;</t>
+          <t>&lt;__main__.DisplayOutputs object at 0x7fcda8314e50&gt;</t>
         </is>
       </c>
       <c r="B108" t="n">
-        <v>0.9375</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>&lt;__main__.DisplayOutputs object at 0x7f38b41323d0&gt;</t>
+          <t>&lt;__main__.DisplayOutputs object at 0x7fcda8314e50&gt;</t>
         </is>
       </c>
       <c r="B109" t="n">
-        <v>0.9375</v>
+        <v>0.734375</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>&lt;__main__.DisplayOutputs object at 0x7f38b41323d0&gt;</t>
+          <t>&lt;__main__.DisplayOutputs object at 0x7fcda8314e50&gt;</t>
         </is>
       </c>
       <c r="B110" t="n">
-        <v>0.96875</v>
+        <v>0.8125</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>&lt;__main__.DisplayOutputs object at 0x7f38b41323d0&gt;</t>
+          <t>&lt;__main__.DisplayOutputs object at 0x7fcda8314e50&gt;</t>
         </is>
       </c>
       <c r="B111" t="n">
-        <v>0.96875</v>
+        <v>0.8125</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>&lt;__main__.DisplayOutputs object at 0x7f38b41323d0&gt;</t>
+          <t>&lt;__main__.DisplayOutputs object at 0x7fcda8314e50&gt;</t>
         </is>
       </c>
       <c r="B112" t="n">
-        <v>0.96875</v>
+        <v>0.765625</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>&lt;__main__.DisplayOutputs object at 0x7f38b41323d0&gt;</t>
+          <t>&lt;__main__.DisplayOutputs object at 0x7fcda8314e50&gt;</t>
         </is>
       </c>
       <c r="B113" t="n">
-        <v>0.953125</v>
+        <v>0.796875</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>&lt;__main__.DisplayOutputs object at 0x7f38b41323d0&gt;</t>
+          <t>&lt;__main__.DisplayOutputs object at 0x7fcda8314e50&gt;</t>
         </is>
       </c>
       <c r="B114" t="n">
-        <v>1</v>
+        <v>0.703125</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>&lt;__main__.DisplayOutputs object at 0x7fcda8314e50&gt;</t>
+        </is>
+      </c>
+      <c r="B115" t="n">
+        <v>0.828125</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>&lt;__main__.DisplayOutputs object at 0x7fcda8314e50&gt;</t>
+        </is>
+      </c>
+      <c r="B116" t="n">
+        <v>0.796875</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>&lt;__main__.DisplayOutputs object at 0x7fcda8314e50&gt;</t>
+        </is>
+      </c>
+      <c r="B117" t="n">
+        <v>0.828125</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>&lt;__main__.DisplayOutputs object at 0x7fcda8314e50&gt;</t>
+        </is>
+      </c>
+      <c r="B118" t="n">
+        <v>0.7377049180327869</v>
       </c>
     </row>
   </sheetData>

</xml_diff>